<commit_message>
migrasi engine export excel
</commit_message>
<xml_diff>
--- a/assets/template/1-1.xlsx
+++ b/assets/template/1-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\e-borang\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ridho\xampp7.4.25\htdocs\borangft\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FE5E34-BE85-4B1C-8318-143E50EC2324}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA2C51-B5D6-481F-8AA8-AC9D809466A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="3795" windowWidth="19680" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-2025" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-1" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -289,6 +289,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,12 +721,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3:XFD3"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,6 +995,486 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>